<commit_message>
DM Cube Skeleton now using RDFCubeWorkbook.xlsx instead of the .csv file. Fixes error of missing column in the .XLSX and some  var name issues. Successfully creates the cube.
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="24540" windowHeight="12720"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="24540" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
   <si>
     <t>prefix</t>
   </si>
@@ -312,6 +312,24 @@
   </si>
   <si>
     <t>Create RDF Data cubes for Clinical Results Data</t>
+  </si>
+  <si>
+    <t>codeType</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>SDTM</t>
+  </si>
+  <si>
+    <t>nciDomainValue</t>
+  </si>
+  <si>
+    <t>C66731</t>
+  </si>
+  <si>
+    <t>C74457</t>
   </si>
 </sst>
 </file>
@@ -804,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -884,259 +902,318 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="7" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="65.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1147,200 +1224,243 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD20"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1349,200 +1469,243 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cube output to /data folder within package. Use of var domainName to specify "demog" in multiple places instead of hard coding. Should become parameter later. Workbook sheet name changed to demog-Components from DM-Components.
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
-    <sheet name="DM-Components" sheetId="3" r:id="rId2"/>
+    <sheet name="demog-Components" sheetId="3" r:id="rId2"/>
     <sheet name="AE-Components" sheetId="5" r:id="rId3"/>
     <sheet name="XX-Components" sheetId="6" r:id="rId4"/>
     <sheet name="CubePrefixes" sheetId="4" r:id="rId5"/>
@@ -905,7 +905,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
domainName var is hard coded. Should become a parameter.  (see ~ 97)
Attaching the cube metadata from Workbook instead of hard coded. Need some help streamlining the inefficient steps prior to qb.buildDSD call. : see comments in that section.
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
   <si>
     <t>prefix</t>
   </si>
@@ -209,9 +209,6 @@
     <t>DC-Demog-R-V</t>
   </si>
   <si>
-    <t>Cube name prefix (will be appended with version number by script</t>
-  </si>
-  <si>
     <t>createdBy</t>
   </si>
   <si>
@@ -330,13 +327,23 @@
   </si>
   <si>
     <t>C74457</t>
+  </si>
+  <si>
+    <t>Cube name prefix (will be appended with version number by script
+No. Will be set in code based on domainName paramter</t>
+  </si>
+  <si>
+    <t>Demographics Analysis Results</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +424,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -479,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -512,6 +534,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -834,59 +860,59 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -902,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,10 +951,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>36</v>
@@ -945,7 +971,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6" t="s">
@@ -961,10 +987,10 @@
         <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>41</v>
@@ -979,7 +1005,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="6" t="s">
@@ -995,7 +1021,7 @@
         <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
@@ -1011,7 +1037,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="6" t="s">
@@ -1027,10 +1053,10 @@
         <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>49</v>
@@ -1095,130 +1121,145 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>63</v>
+      <c r="F12" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="6" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1241,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,10 +1293,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>36</v>
@@ -1368,7 +1409,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>61</v>
@@ -1380,10 +1421,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1392,10 +1433,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1404,10 +1445,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1416,10 +1457,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1428,10 +1469,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1440,10 +1481,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1452,10 +1493,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1486,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1497,10 +1538,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>36</v>
@@ -1613,7 +1654,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>61</v>
@@ -1625,10 +1666,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1637,10 +1678,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1649,10 +1690,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1661,10 +1702,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1673,10 +1714,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1685,10 +1726,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1697,10 +1738,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>

</xml_diff>

<commit_message>
Using DM instead of "demog" for cube name, paths in prefixes, etc.   Use of standard SDTM domain names for consistency across data sets.
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
-    <sheet name="demog-Components" sheetId="3" r:id="rId2"/>
+    <sheet name="DM-Components" sheetId="3" r:id="rId2"/>
     <sheet name="AE-Components" sheetId="5" r:id="rId3"/>
     <sheet name="XX-Components" sheetId="6" r:id="rId4"/>
     <sheet name="CubePrefixes" sheetId="4" r:id="rId5"/>
@@ -47,9 +47,6 @@
     <t>dccs</t>
   </si>
   <si>
-    <t>http://www.example.org/dc/demog/dccs/</t>
-  </si>
-  <si>
     <t>dct</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>ds</t>
   </si>
   <si>
-    <t>http://www.example.org/dc/demog/dataset/</t>
-  </si>
-  <si>
     <t>mms</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>prop</t>
   </si>
   <si>
-    <t>http://www.example.org/dc/demog/prop/</t>
-  </si>
-  <si>
     <t>prov</t>
   </si>
   <si>
@@ -206,9 +197,6 @@
     <t>dataCubeFileName</t>
   </si>
   <si>
-    <t>DC-Demog-R-V</t>
-  </si>
-  <si>
     <t>createdBy</t>
   </si>
   <si>
@@ -258,9 +246,6 @@
   </si>
   <si>
     <t>demog.AR.csv</t>
-  </si>
-  <si>
-    <t>Data source (obsFileName)</t>
   </si>
   <si>
     <t>metadata</t>
@@ -337,6 +322,21 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>http://www.example.org/dc/DM/dccs/</t>
+  </si>
+  <si>
+    <t>http://www.example.org/dc/DM/dataset/</t>
+  </si>
+  <si>
+    <t>http://www.example.org/dc/DM/prop/</t>
+  </si>
+  <si>
+    <t>DC-DM-R-V</t>
+  </si>
+  <si>
+    <t>Data source (obsFileName). Set this programmtically based on name of input file!</t>
   </si>
 </sst>
 </file>
@@ -860,59 +860,59 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +931,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,316 +945,316 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="20" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1282,32 +1282,32 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1433,10 +1433,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1445,10 +1445,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1469,10 +1469,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1527,32 +1527,32 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1654,10 +1654,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1666,10 +1666,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1678,10 +1678,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1690,10 +1690,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1702,10 +1702,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1755,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,119 +1800,107 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CubeWorkbook sheet "CubePrefixes" now used instead of DMCubePrefixes.csv and CommonCubePrefixes.csv.  Common prefixes come from the Workbook. Custom ones for the domain (/dccs/, /dataset/, and /prop/) are formed using the domainName specified within the R code. Also fixes error of using AE prefixes (.../ae/dccs/) etc. from prior work.
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="24540" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="24540" windowHeight="12720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
   <si>
     <t>prefix</t>
   </si>
@@ -44,18 +44,12 @@
     <t>http://www.w3.org/ns/dcat#</t>
   </si>
   <si>
-    <t>dccs</t>
-  </si>
-  <si>
     <t>dct</t>
   </si>
   <si>
     <t>http://purl.org/dc/terms/</t>
   </si>
   <si>
-    <t>ds</t>
-  </si>
-  <si>
     <t>mms</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
   </si>
   <si>
     <t>http://purl.org/pav</t>
-  </si>
-  <si>
-    <t>prop</t>
   </si>
   <si>
     <t>prov</t>
@@ -322,15 +313,6 @@
   </si>
   <si>
     <t>title</t>
-  </si>
-  <si>
-    <t>http://www.example.org/dc/DM/dccs/</t>
-  </si>
-  <si>
-    <t>http://www.example.org/dc/DM/dataset/</t>
-  </si>
-  <si>
-    <t>http://www.example.org/dc/DM/prop/</t>
   </si>
   <si>
     <t>DC-DM-R-V</t>
@@ -860,59 +842,59 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -945,316 +927,316 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E1" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="20" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1282,32 +1264,32 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1317,7 +1299,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1327,7 +1309,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1337,7 +1319,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1347,7 +1329,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1357,7 +1339,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1367,7 +1349,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1377,7 +1359,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1387,7 +1369,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1397,10 +1379,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1409,10 +1391,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1421,10 +1403,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1433,10 +1415,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1445,10 +1427,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1457,10 +1439,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1469,10 +1451,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1481,10 +1463,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1493,10 +1475,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1527,32 +1509,32 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1562,7 +1544,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1572,7 +1554,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1582,7 +1564,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1592,7 +1574,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1602,7 +1584,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1612,7 +1594,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1622,7 +1604,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1632,7 +1614,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1642,10 +1624,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1654,10 +1636,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1666,10 +1648,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1678,10 +1660,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1690,10 +1672,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1702,10 +1684,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1714,10 +1696,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1726,10 +1708,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1738,10 +1720,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1755,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,106 +1782,82 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added specification for AE table
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
   <si>
     <t>RDF Data Cube Workbook for BUildCube.R</t>
   </si>
@@ -48,7 +48,7 @@
     <t>XX-Components</t>
   </si>
   <si>
-    <t>Specify the dimensions, measure, attributes, and cube metadata for each cube (XX).  </t>
+    <t>Specify the dimensions, measure, attributes, and cube metadata for each cube (XX).</t>
   </si>
   <si>
     <t>CubePrefixes</t>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>obsFileName</t>
+  </si>
+  <si>
+    <t>dm.AR.csv</t>
   </si>
   <si>
     <t>dataCubeFileName</t>
@@ -178,7 +181,7 @@
     <t>0.5.2</t>
   </si>
   <si>
-    <t>Version of cube with format n.n.n </t>
+    <t>Version of cube with format n.n.n</t>
   </si>
   <si>
     <t>createdBy</t>
@@ -232,13 +235,73 @@
     <t>Data source (obsFileName). Set this programmtically based on name of input file!</t>
   </si>
   <si>
-    <t>AE domain/cube, modeled after DM-COMPONENTS</t>
+    <t>domainName</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>The domain name, also part of the spreadsheet tab name</t>
+  </si>
+  <si>
+    <t>obsFileNameDirectory</t>
+  </si>
+  <si>
+    <t>!example</t>
+  </si>
+  <si>
+    <t>The directory containd the wasDerivedFrom file</t>
+  </si>
+  <si>
+    <t>dataCubeOutDirectory</t>
+  </si>
+  <si>
+    <t>!temporary</t>
+  </si>
+  <si>
+    <t>trta</t>
+  </si>
+  <si>
+    <t>aesoc</t>
+  </si>
+  <si>
+    <t>System Organ Class</t>
+  </si>
+  <si>
+    <t>aedecod</t>
+  </si>
+  <si>
+    <t>Preferred Term</t>
+  </si>
+  <si>
+    <t>https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae.xpt</t>
+  </si>
+  <si>
+    <t>ae.AR.csv</t>
+  </si>
+  <si>
+    <t>DC-AE-R-V</t>
+  </si>
+  <si>
+    <t>Cube with 6 dimensions and 1 measure (measure)</t>
+  </si>
+  <si>
+    <t>Adverse event sample table </t>
+  </si>
+  <si>
+    <t>Adverse Event Analysis Results</t>
+  </si>
+  <si>
+    <t>Adverse Events results data set</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>Pages for additional domains, modeled after DM-COMPONENTS</t>
   </si>
   <si>
     <t>??</t>
-  </si>
-  <si>
-    <t>Pages for additional domains, modeled after DM-COMPONENTS</t>
   </si>
   <si>
     <t>prefix</t>
@@ -515,7 +578,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -578,6 +641,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -714,6 +781,12 @@
       </c>
       <c r="C3" s="0"/>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0"/>
+    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>3</v>
@@ -779,10 +852,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -981,25 +1054,27 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="F12" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
+      <c r="A13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18" t="s">
         <v>49</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,15 +1082,15 @@
         <v>43</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,15 +1098,15 @@
         <v>43</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,15 +1114,15 @@
         <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,12 +1130,12 @@
         <v>43</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F17" s="11"/>
     </row>
@@ -1069,12 +1144,12 @@
         <v>43</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -1083,12 +1158,12 @@
         <v>43</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -1097,12 +1172,12 @@
         <v>43</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F20" s="11"/>
     </row>
@@ -1111,15 +1186,54 @@
         <v>43</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="17" t="s">
         <v>69</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1141,10 +1255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1156,230 +1270,377 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="10"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="10"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1411,24 +1672,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>72</v>
+      <c r="A1" s="19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -1527,7 +1788,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>46</v>
@@ -1542,7 +1803,7 @@
         <v>43</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1554,7 +1815,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1566,7 +1827,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1578,7 +1839,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1590,7 +1851,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1602,7 +1863,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1614,7 +1875,7 @@
         <v>43</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1626,7 +1887,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1664,114 +1925,114 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>76</v>
+      <c r="A2" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>78</v>
+      <c r="A3" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>80</v>
+      <c r="A4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>82</v>
+      <c r="A5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>84</v>
+      <c r="A6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>86</v>
+      <c r="A7" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>88</v>
+      <c r="A8" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>90</v>
+      <c r="A9" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>92</v>
+      <c r="A10" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>94</v>
+      <c r="A11" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>96</v>
+      <c r="A12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>98</v>
+      <c r="A13" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>100</v>
+      <c r="A14" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AE-Components with dummy value in otherwise empty column
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="123">
   <si>
     <t>RDF Data Cube Workbook for BUildCube.R</t>
   </si>
@@ -286,7 +286,7 @@
     <t>Cube with 6 dimensions and 1 measure (measure)</t>
   </si>
   <si>
-    <t>Adverse event sample table </t>
+    <t>Adverse event sample table</t>
   </si>
   <si>
     <t>Adverse Event Analysis Results</t>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>AE</t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
   <si>
     <t>Pages for additional domains, modeled after DM-COMPONENTS</t>
@@ -1255,13 +1258,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65536"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7091836734694"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.2857142857143"/>
@@ -1631,15 +1634,17 @@
       <c r="B24" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae"/>
+    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae.xpt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1673,7 +1678,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1793,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>46</v>
@@ -1925,114 +1930,114 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prefix for rrdfqbcrnd0
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="125">
   <si>
     <t>RDF Data Cube Workbook for BUildCube.R</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>http://www.w3.org/2001/XMLSchema#</t>
+  </si>
+  <si>
+    <t>rrdfqbcrnd0</t>
+  </si>
+  <si>
+    <t>http://www.example.org/rrdfqbcrnd0/</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1266,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1915,10 +1921,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2040,7 +2046,18 @@
         <v>122</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" display="http://www.example.org/rrdfqbcrnd0/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update workbook to containt DEMO
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="417"/>
   </bookViews>
   <sheets>
-    <sheet name="Intro" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DM-Components" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AE-Components" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="XX-Components" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CubePrefixes" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="DEMO-Components" sheetId="6" r:id="rId1"/>
+    <sheet name="Intro" sheetId="1" r:id="rId2"/>
+    <sheet name="DM-Components" sheetId="2" r:id="rId3"/>
+    <sheet name="AE-Components" sheetId="3" r:id="rId4"/>
+    <sheet name="XX-Components" sheetId="4" r:id="rId5"/>
+    <sheet name="CubePrefixes" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="128">
   <si>
     <t>RDF Data Cube Workbook for BUildCube.R</t>
   </si>
@@ -395,16 +395,22 @@
   </si>
   <si>
     <t>http://www.example.org/rrdfqbcrnd0/</t>
+  </si>
+  <si>
+    <t>demo.AR.csv</t>
+  </si>
+  <si>
+    <t>ethnic</t>
+  </si>
+  <si>
+    <t>Ethnic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -413,22 +419,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -436,7 +427,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -444,7 +435,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -452,8 +443,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -461,7 +452,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -469,7 +460,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -477,7 +468,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -485,7 +476,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
@@ -493,7 +484,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -508,7 +499,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="14"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
@@ -537,159 +528,93 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -748,61 +673,764 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E12" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="83.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="83.5703125" style="1"/>
+    <col min="4" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -810,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -818,7 +1446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -826,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -834,8 +1462,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -846,37 +1474,27 @@
     <hyperlink ref="B9" location="'XX-Components'!A1" display="XX-Components"/>
     <hyperlink ref="B10" location="CubePrefixes!A1" display="CubePrefixes"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="55.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="12.7109375"/>
+    <col min="2" max="4" width="18.28515625"/>
+    <col min="5" max="5" width="65.5703125" style="1"/>
+    <col min="6" max="6" width="55.7109375" style="1"/>
+    <col min="7" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -896,7 +1514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
@@ -912,7 +1530,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -922,7 +1540,7 @@
       <c r="C3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -930,7 +1548,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -946,7 +1564,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -962,7 +1580,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -978,7 +1596,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
@@ -988,7 +1606,7 @@
       <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -996,7 +1614,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -1010,7 +1628,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -1024,7 +1642,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
@@ -1038,7 +1656,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -1054,7 +1672,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>43</v>
       </c>
@@ -1070,7 +1688,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>43</v>
       </c>
@@ -1086,7 +1704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -1102,7 +1720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -1118,7 +1736,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
@@ -1134,7 +1752,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1148,7 +1766,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>43</v>
       </c>
@@ -1162,7 +1780,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>43</v>
       </c>
@@ -1176,7 +1794,7 @@
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>
@@ -1190,7 +1808,7 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>43</v>
       </c>
@@ -1206,11 +1824,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
         <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1220,11 +1838,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -1234,11 +1852,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="0" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
         <v>77</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1247,39 +1865,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adsl.xpt"/>
+    <hyperlink ref="E11" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="11.7109375"/>
+    <col min="2" max="4" width="18.28515625"/>
+    <col min="5" max="5" width="65.5703125"/>
+    <col min="6" max="6" width="41"/>
+    <col min="7" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1299,7 +1909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
@@ -1315,7 +1925,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -1331,7 +1941,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -1347,7 +1957,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1973,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -1379,7 +1989,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +2005,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +2019,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -1423,7 +2033,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
@@ -1437,7 +2047,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -1453,7 +2063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>43</v>
       </c>
@@ -1469,7 +2079,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>43</v>
       </c>
@@ -1485,7 +2095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +2111,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -1517,7 +2127,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
@@ -1533,7 +2143,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1547,7 +2157,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>43</v>
       </c>
@@ -1561,7 +2171,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>43</v>
       </c>
@@ -1575,7 +2185,7 @@
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>
@@ -1589,7 +2199,7 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>43</v>
       </c>
@@ -1605,11 +2215,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
         <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1619,11 +2229,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -1633,14 +2243,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="0" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1650,44 +2260,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae.xpt"/>
+    <hyperlink ref="E11" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="12"/>
+    <col min="2" max="4" width="18.28515625"/>
+    <col min="5" max="5" width="23.140625"/>
+    <col min="6" max="6" width="26.85546875"/>
+    <col min="7" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
@@ -1707,7 +2309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -1717,7 +2319,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -1727,7 +2329,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -1737,7 +2339,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -1747,7 +2349,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
@@ -1757,7 +2359,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
@@ -1767,7 +2369,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +2379,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
@@ -1787,7 +2389,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>38</v>
       </c>
@@ -1797,7 +2399,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>94</v>
       </c>
@@ -1809,7 +2411,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +2423,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -1833,7 +2435,7 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -1845,7 +2447,7 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
@@ -1857,7 +2459,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1869,7 +2471,7 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +2483,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>43</v>
       </c>
@@ -1893,7 +2495,7 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>
@@ -1906,35 +2508,27 @@
       <c r="F20" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="43.42578125"/>
+    <col min="3" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>95</v>
       </c>
@@ -1942,7 +2536,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>97</v>
       </c>
@@ -1950,7 +2544,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>99</v>
       </c>
@@ -1958,7 +2552,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>101</v>
       </c>
@@ -1966,7 +2560,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>103</v>
       </c>
@@ -1974,7 +2568,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>105</v>
       </c>
@@ -1982,7 +2576,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>107</v>
       </c>
@@ -1990,7 +2584,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>109</v>
       </c>
@@ -1998,7 +2592,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>111</v>
       </c>
@@ -2006,7 +2600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>113</v>
       </c>
@@ -2014,7 +2608,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>115</v>
       </c>
@@ -2022,7 +2616,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>117</v>
       </c>
@@ -2030,7 +2624,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>119</v>
       </c>
@@ -2038,7 +2632,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>121</v>
       </c>
@@ -2046,8 +2640,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>123</v>
       </c>
       <c r="B15" s="22" t="s">
@@ -2056,14 +2650,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" display="http://www.example.org/rrdfqbcrnd0/"/>
+    <hyperlink ref="B15" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Export of SAS to csv updated
</commit_message>
<xml_diff>
--- a/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="DEMO-Components" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Intro" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="DM-Components" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="AE-Components" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="XX-Components" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CubePrefixes" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="DEMO-Components" sheetId="1" r:id="rId1"/>
+    <sheet name="Intro" sheetId="2" r:id="rId2"/>
+    <sheet name="DM-Components" sheetId="3" r:id="rId3"/>
+    <sheet name="AE-Components" sheetId="4" r:id="rId4"/>
+    <sheet name="XX-Components" sheetId="5" r:id="rId5"/>
+    <sheet name="CubePrefixes" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="138">
   <si>
     <t>compType</t>
   </si>
@@ -49,7 +48,7 @@
     <t>DATA</t>
   </si>
   <si>
-    <t> </t>
+    <t/>
   </si>
   <si>
     <t>Treatment Arm</t>
@@ -432,16 +431,16 @@
   </si>
   <si>
     <t>http://www.example.org/rrdfqbcrnd0/</t>
+  </si>
+  <si>
+    <t>Cube name prefix (will be appended with version number by script. --&gt; No. Will be set in code based on domainName parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -450,22 +449,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -473,7 +457,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -481,7 +465,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -489,7 +473,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
@@ -497,7 +481,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -512,7 +496,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -520,7 +504,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -528,8 +512,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -537,7 +521,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -545,7 +529,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="14"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
@@ -574,159 +558,91 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -785,34 +701,329 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="8:8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.75510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="10.85546875"/>
+    <col min="2" max="2" width="20.140625"/>
+    <col min="3" max="3" width="9.7109375"/>
+    <col min="4" max="4" width="15.85546875"/>
+    <col min="5" max="5" width="47.28515625"/>
+    <col min="6" max="6" width="81.42578125"/>
+    <col min="7" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,7 +1043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -852,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -870,7 +1081,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -886,7 +1097,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -902,7 +1113,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -920,7 +1131,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -935,7 +1146,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -950,7 +1161,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -966,7 +1177,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -980,7 +1191,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -994,7 +1205,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -1010,7 +1221,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -1026,7 +1237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>34</v>
       </c>
@@ -1039,10 +1250,10 @@
         <v>40</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -1058,7 +1269,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
@@ -1074,7 +1285,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
@@ -1090,7 +1301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -1104,7 +1315,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -1118,7 +1329,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -1132,7 +1343,7 @@
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -1146,7 +1357,7 @@
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>34</v>
       </c>
@@ -1162,7 +1373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1178,7 +1389,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1194,7 +1405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>34</v>
       </c>
@@ -1210,12 +1421,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adsl.xpt"/>
+    <hyperlink ref="E12" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1223,60 +1433,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="8:8 A12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" activeCellId="1" sqref="A8:XFD8 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="83.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="6" width="8.70918367346939"/>
+    <col min="1" max="1" width="8.7109375" style="6"/>
+    <col min="2" max="2" width="16.85546875" style="6"/>
+    <col min="3" max="3" width="83.5703125" style="11"/>
+    <col min="4" max="1025" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="0"/>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
+      <c r="B1"/>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2"/>
       <c r="B2" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3"/>
       <c r="B3" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7"/>
       <c r="B7" s="17" t="s">
         <v>73</v>
       </c>
@@ -1284,8 +1491,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8"/>
       <c r="B8" s="17" t="s">
         <v>75</v>
       </c>
@@ -1293,8 +1500,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9"/>
       <c r="B9" s="17" t="s">
         <v>77</v>
       </c>
@@ -1302,8 +1509,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10"/>
       <c r="B10" s="17" t="s">
         <v>79</v>
       </c>
@@ -1311,13 +1518,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
@@ -1329,37 +1536,29 @@
     <hyperlink ref="B9" location="'XX-Components'!A1" display="XX-Components"/>
     <hyperlink ref="B10" location="CubePrefixes!A1" display="CubePrefixes"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="8:8 A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCellId="1" sqref="A8:XFD8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="55.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col min="1" max="1" width="12.7109375" style="6"/>
+    <col min="2" max="4" width="18.28515625" style="6"/>
+    <col min="5" max="5" width="65.5703125" style="11"/>
+    <col min="6" max="6" width="55.7109375" style="11"/>
+    <col min="7" max="1025" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1395,7 +1594,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1612,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1429,7 +1628,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1445,7 +1644,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1660,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1479,7 +1678,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -1493,7 +1692,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
@@ -1507,7 +1706,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -1521,7 +1720,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
@@ -1537,7 +1736,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -1553,7 +1752,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>34</v>
       </c>
@@ -1569,7 +1768,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -1585,7 +1784,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -1601,7 +1800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
@@ -1617,7 +1816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
@@ -1631,7 +1830,7 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -1645,7 +1844,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -1659,7 +1858,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -1673,7 +1872,7 @@
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -1689,7 +1888,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
@@ -1703,7 +1902,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1717,7 +1916,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1730,39 +1929,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adsl.xpt"/>
+    <hyperlink ref="E11" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="1" sqref="8:8 D24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" activeCellId="1" sqref="A8:XFD8 D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="41"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col min="1" max="1" width="11.7109375" style="6"/>
+    <col min="2" max="4" width="18.28515625" style="6"/>
+    <col min="5" max="5" width="65.5703125" style="6"/>
+    <col min="6" max="6" width="41" style="6"/>
+    <col min="7" max="1025" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1782,7 +1973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1989,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1814,7 +2005,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1830,7 +2021,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1846,7 +2037,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1862,7 +2053,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1878,7 +2069,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -1892,7 +2083,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +2097,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -1920,7 +2111,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
@@ -1936,7 +2127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -1952,7 +2143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>34</v>
       </c>
@@ -1968,7 +2159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -1984,7 +2175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -2000,7 +2191,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
@@ -2016,7 +2207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
@@ -2030,7 +2221,7 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -2044,7 +2235,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -2058,7 +2249,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -2072,7 +2263,7 @@
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -2088,14 +2279,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="0"/>
+      <c r="D22"/>
       <c r="E22" s="11" t="s">
         <v>103</v>
       </c>
@@ -2103,14 +2294,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="0"/>
+      <c r="D23"/>
       <c r="E23" s="11" t="s">
         <v>65</v>
       </c>
@@ -2118,7 +2309,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -2135,49 +2326,41 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" display="https://phuse-scripts.googlecode.com/svn/trunk/scriptathon2014/data/adae.xpt"/>
+    <hyperlink ref="E11" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="1" sqref="8:8 B41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" activeCellId="1" sqref="A8:XFD8 B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="26.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col min="1" max="1" width="12" style="6"/>
+    <col min="2" max="4" width="18.28515625" style="6"/>
+    <col min="5" max="5" width="23.140625" style="6"/>
+    <col min="6" max="6" width="26.85546875" style="6"/>
+    <col min="7" max="1025" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -2197,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2207,7 +2390,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2217,7 +2400,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2227,7 +2410,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2237,7 +2420,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2247,7 +2430,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2257,7 +2440,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
@@ -2267,7 +2450,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2460,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -2287,7 +2470,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>106</v>
       </c>
@@ -2299,7 +2482,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
@@ -2311,7 +2494,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -2323,7 +2506,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -2335,7 +2518,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
@@ -2347,7 +2530,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
@@ -2359,7 +2542,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
@@ -2371,7 +2554,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -2383,7 +2566,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -2396,35 +2579,27 @@
       <c r="F20" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="8:8 B19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" activeCellId="1" sqref="A8:XFD8 B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="43.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="6" width="8.70918367346939"/>
+    <col min="1" max="1" width="8.7109375" style="6"/>
+    <col min="2" max="2" width="43.42578125" style="6"/>
+    <col min="3" max="1025" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -2432,7 +2607,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>109</v>
       </c>
@@ -2440,7 +2615,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>111</v>
       </c>
@@ -2448,7 +2623,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>113</v>
       </c>
@@ -2456,7 +2631,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>115</v>
       </c>
@@ -2464,7 +2639,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>117</v>
       </c>
@@ -2472,7 +2647,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -2480,7 +2655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>121</v>
       </c>
@@ -2488,7 +2663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>123</v>
       </c>
@@ -2496,7 +2671,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>125</v>
       </c>
@@ -2504,7 +2679,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>127</v>
       </c>
@@ -2512,7 +2687,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>129</v>
       </c>
@@ -2520,7 +2695,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>131</v>
       </c>
@@ -2528,7 +2703,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>133</v>
       </c>
@@ -2536,7 +2711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>135</v>
       </c>
@@ -2546,14 +2721,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" display="http://www.example.org/rrdfqbcrnd0/"/>
+    <hyperlink ref="B15" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>